<commit_message>
Added all basic stats
</commit_message>
<xml_diff>
--- a/src/lib/excels/CI_Comps.xlsx
+++ b/src/lib/excels/CI_Comps.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F855C4D-0E57-4374-A1C4-F1610B780E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0F855C4D-0E57-4374-A1C4-F1610B780E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45FDD9A5-0F5D-1E43-8A00-1571EFB0A6FF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17664" xr2:uid="{AB0D5E22-6F5B-EC43-9578-14FEE2B3982A}"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{AB0D5E22-6F5B-EC43-9578-14FEE2B3982A}"/>
   </bookViews>
   <sheets>
     <sheet name="CIs" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="254">
   <si>
     <t>Packaged</t>
   </si>
@@ -790,6 +790,9 @@
   </si>
   <si>
     <t>Final Price</t>
+  </si>
+  <si>
+    <t>Not controllable</t>
   </si>
 </sst>
 </file>
@@ -921,7 +924,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
@@ -1113,7 +1116,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1413,62 +1416,62 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH3" sqref="AH3"/>
+      <selection pane="topRight" activeCell="AF16" sqref="AF16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.296875" customWidth="1"/>
-    <col min="10" max="10" width="24.19921875" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" customWidth="1"/>
+    <col min="10" max="10" width="24.1640625" customWidth="1"/>
     <col min="11" max="11" width="8" customWidth="1"/>
     <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="43.69921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.69921875" customWidth="1"/>
-    <col min="16" max="16" width="23.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.19921875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
+    <col min="16" max="16" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.69921875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.69921875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.19921875" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="19.69921875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.296875" customWidth="1"/>
+    <col min="25" max="25" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" customWidth="1"/>
     <col min="30" max="30" width="24.5" customWidth="1"/>
-    <col min="31" max="31" width="10.796875" customWidth="1"/>
-    <col min="32" max="32" width="13.296875" customWidth="1"/>
-    <col min="33" max="33" width="11.796875" customWidth="1"/>
+    <col min="31" max="31" width="10.83203125" customWidth="1"/>
+    <col min="32" max="32" width="13.33203125" customWidth="1"/>
+    <col min="33" max="33" width="11.83203125" customWidth="1"/>
     <col min="34" max="34" width="12" customWidth="1"/>
     <col min="37" max="37" width="22.5" customWidth="1"/>
-    <col min="38" max="38" width="27.69921875" customWidth="1"/>
-    <col min="40" max="40" width="19.19921875" customWidth="1"/>
-    <col min="41" max="41" width="33.296875" customWidth="1"/>
-    <col min="42" max="42" width="24.796875" customWidth="1"/>
-    <col min="43" max="43" width="19.19921875" customWidth="1"/>
-    <col min="44" max="44" width="11.69921875" customWidth="1"/>
+    <col min="38" max="38" width="27.6640625" customWidth="1"/>
+    <col min="40" max="40" width="19.1640625" customWidth="1"/>
+    <col min="41" max="41" width="33.33203125" customWidth="1"/>
+    <col min="42" max="42" width="24.83203125" customWidth="1"/>
+    <col min="43" max="43" width="19.1640625" customWidth="1"/>
+    <col min="44" max="44" width="11.6640625" customWidth="1"/>
     <col min="45" max="45" width="31" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="25.19921875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="20" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="26.796875" customWidth="1"/>
-    <col min="50" max="50" width="24.796875" customWidth="1"/>
-    <col min="51" max="51" width="20.19921875" customWidth="1"/>
-    <col min="52" max="52" width="28.796875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="26.83203125" customWidth="1"/>
+    <col min="50" max="50" width="24.83203125" customWidth="1"/>
+    <col min="51" max="51" width="20.1640625" customWidth="1"/>
+    <col min="52" max="52" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="27" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="25" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1587,7 +1590,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1805,7 +1808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1922,7 +1925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2039,7 +2042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -2156,7 +2159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -2273,7 +2276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -2392,7 +2395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -2512,7 +2515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -2631,7 +2634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -2750,7 +2753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>243</v>
       </c>
@@ -2868,7 +2871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>243</v>
       </c>
@@ -2989,7 +2992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>243</v>
       </c>
@@ -3110,7 +3113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
@@ -3230,7 +3233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
@@ -3348,7 +3351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
@@ -3466,7 +3469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -3583,7 +3586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
@@ -3700,7 +3703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -3817,7 +3820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -3934,7 +3937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
@@ -4051,7 +4054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
@@ -4146,9 +4149,11 @@
         <v>0</v>
       </c>
       <c r="AF23" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="AG23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AG23" s="2"/>
       <c r="AH23" t="s">
         <v>4</v>
       </c>
@@ -4168,7 +4173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -4265,9 +4270,11 @@
         <v>0</v>
       </c>
       <c r="AF24" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="AG24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AG24" s="2"/>
       <c r="AH24" t="s">
         <v>4</v>
       </c>
@@ -4287,7 +4294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -4382,9 +4389,11 @@
         <v>8000</v>
       </c>
       <c r="AF25" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="AG25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AG25" s="2"/>
       <c r="AH25" t="s">
         <v>4</v>
       </c>
@@ -4404,7 +4413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -4524,7 +4533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>56</v>
       </c>
@@ -4643,7 +4652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
@@ -4762,7 +4771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -4881,7 +4890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
@@ -5000,7 +5009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>56</v>
       </c>
@@ -5119,7 +5128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>56</v>
       </c>
@@ -5238,7 +5247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>65</v>
       </c>
@@ -5356,7 +5365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
@@ -5474,7 +5483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
@@ -5592,7 +5601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>65</v>
       </c>
@@ -5712,7 +5721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>69</v>
       </c>
@@ -5831,7 +5840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>69</v>
       </c>
@@ -5950,7 +5959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>69</v>
       </c>
@@ -6069,7 +6078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>69</v>
       </c>
@@ -6190,7 +6199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>73</v>
       </c>
@@ -6309,7 +6318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>77</v>
       </c>
@@ -6404,7 +6413,7 @@
         <v>0</v>
       </c>
       <c r="AF42" s="2" t="s">
-        <v>49</v>
+        <v>253</v>
       </c>
       <c r="AG42" s="2" t="s">
         <v>49</v>
@@ -6428,7 +6437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>80</v>
       </c>
@@ -6547,7 +6556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>80</v>
       </c>
@@ -6668,7 +6677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>80</v>
       </c>
@@ -6789,7 +6798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>80</v>
       </c>
@@ -6908,7 +6917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>80</v>
       </c>
@@ -7027,7 +7036,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>84</v>
       </c>
@@ -7146,7 +7155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>87</v>
       </c>
@@ -7265,7 +7274,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>90</v>
       </c>
@@ -7382,7 +7391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>90</v>
       </c>
@@ -7501,7 +7510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>93</v>
       </c>
@@ -7618,7 +7627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>93</v>
       </c>
@@ -7736,7 +7745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>97</v>
       </c>
@@ -7853,7 +7862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>100</v>
       </c>
@@ -7972,7 +7981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>100</v>
       </c>
@@ -8091,7 +8100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>103</v>
       </c>
@@ -8206,7 +8215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>106</v>
       </c>
@@ -8321,7 +8330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>108</v>
       </c>
@@ -8438,7 +8447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>108</v>
       </c>
@@ -8555,7 +8564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>108</v>
       </c>
@@ -8672,7 +8681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>108</v>
       </c>
@@ -8791,7 +8800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Added average prices to stats
</commit_message>
<xml_diff>
--- a/src/lib/excels/CI_Comps.xlsx
+++ b/src/lib/excels/CI_Comps.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{0F855C4D-0E57-4374-A1C4-F1610B780E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45FDD9A5-0F5D-1E43-8A00-1571EFB0A6FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3960B16-8E25-1A4A-BB2A-584F7A9CFA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{AB0D5E22-6F5B-EC43-9578-14FEE2B3982A}"/>
   </bookViews>
@@ -423,9 +423,6 @@
     <t>MaxUsers</t>
   </si>
   <si>
-    <t>PriceExtraUser</t>
-  </si>
-  <si>
     <t xml:space="preserve">CachingPipelineAndDependencies </t>
   </si>
   <si>
@@ -793,6 +790,9 @@
   </si>
   <si>
     <t>Not controllable</t>
+  </si>
+  <si>
+    <t>PriceExtraUser$</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1100,7 @@
     <tableColumn id="34" xr3:uid="{B89B993E-E109-0C41-96BD-143310A5EFC9}" name="PricePerExtraCredit" dataDxfId="12"/>
     <tableColumn id="17" xr3:uid="{61F72404-ABE2-FD43-A410-51C89C6B772D}" name="IncludedUsers" dataDxfId="11"/>
     <tableColumn id="19" xr3:uid="{CF4B76DC-5736-D34A-8FC4-122BBE358245}" name="MaxUsers" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{39310329-028F-A347-AF5A-990BDB186F63}" name="PriceExtraUser" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{39310329-028F-A347-AF5A-990BDB186F63}" name="PriceExtraUser$" dataDxfId="9"/>
     <tableColumn id="36" xr3:uid="{E6BC14CB-2B8D-524E-9B1F-ED6637B2D869}" name="IncludedCreditsPerExtraUser" dataDxfId="8"/>
     <tableColumn id="22" xr3:uid="{0DED0BA4-9DF4-B04C-9035-612BE7063AC5}" name="CachingPipelineAndDependencies " dataDxfId="7"/>
     <tableColumn id="42" xr3:uid="{3EE916D4-D265-2749-A3C4-5B8C674AF706}" name="desc_CachingPipelineAndDependencies" dataDxfId="6"/>
@@ -1415,8 +1415,8 @@
   <dimension ref="A1:AM63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF16" sqref="AF16"/>
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1479,13 +1479,13 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -1500,55 +1500,55 @@
         <v>122</v>
       </c>
       <c r="J1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K1" t="s">
         <v>123</v>
       </c>
       <c r="L1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" t="s">
         <v>144</v>
       </c>
-      <c r="N1" t="s">
-        <v>145</v>
-      </c>
       <c r="O1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P1" t="s">
         <v>124</v>
       </c>
       <c r="Q1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R1" t="s">
         <v>125</v>
       </c>
       <c r="S1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T1" t="s">
         <v>126</v>
       </c>
       <c r="U1" t="s">
+        <v>234</v>
+      </c>
+      <c r="V1" t="s">
         <v>235</v>
       </c>
-      <c r="V1" t="s">
-        <v>236</v>
-      </c>
       <c r="W1" t="s">
+        <v>240</v>
+      </c>
+      <c r="X1" t="s">
+        <v>239</v>
+      </c>
+      <c r="Y1" t="s">
         <v>241</v>
       </c>
-      <c r="X1" t="s">
-        <v>240</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>242</v>
-      </c>
       <c r="Z1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AA1" t="s">
         <v>127</v>
@@ -1560,34 +1560,34 @@
         <v>129</v>
       </c>
       <c r="AD1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF1" t="s">
         <v>130</v>
       </c>
-      <c r="AE1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
+        <v>217</v>
+      </c>
+      <c r="AH1" t="s">
         <v>131</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>218</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>132</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>219</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>133</v>
       </c>
-      <c r="AK1" t="s">
-        <v>220</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>134</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
@@ -1601,10 +1601,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1616,79 +1616,79 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" t="s">
         <v>148</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>149</v>
       </c>
-      <c r="M2" t="s">
-        <v>150</v>
-      </c>
       <c r="N2" t="s">
+        <v>246</v>
+      </c>
+      <c r="O2" t="s">
+        <v>232</v>
+      </c>
+      <c r="P2" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>230</v>
+      </c>
+      <c r="R2" t="s">
+        <v>248</v>
+      </c>
+      <c r="S2" t="s">
         <v>247</v>
       </c>
-      <c r="O2" t="s">
+      <c r="T2" t="s">
+        <v>249</v>
+      </c>
+      <c r="U2" t="s">
         <v>233</v>
       </c>
-      <c r="P2" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>231</v>
-      </c>
-      <c r="R2" t="s">
-        <v>249</v>
-      </c>
-      <c r="S2" t="s">
-        <v>248</v>
-      </c>
-      <c r="T2" t="s">
-        <v>250</v>
-      </c>
-      <c r="U2" t="s">
-        <v>234</v>
-      </c>
       <c r="V2" t="s">
+        <v>236</v>
+      </c>
+      <c r="W2" t="s">
         <v>237</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>238</v>
       </c>
-      <c r="X2" t="s">
-        <v>239</v>
-      </c>
       <c r="Y2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AA2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AB2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AC2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AD2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AF2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AH2" t="s">
         <v>26</v>
       </c>
       <c r="AJ2" t="s">
+        <v>226</v>
+      </c>
+      <c r="AL2" t="s">
         <v>227</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>228</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.2">
@@ -1724,7 +1724,7 @@
         <v>1800</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>20</v>
@@ -1787,7 +1787,7 @@
         <v>4</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AH3" t="s">
         <v>4</v>
@@ -1841,7 +1841,7 @@
         <v>52</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>119</v>
@@ -1904,7 +1904,7 @@
         <v>4</v>
       </c>
       <c r="AG4" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AH4" t="s">
         <v>4</v>
@@ -1958,7 +1958,7 @@
         <v>52</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>119</v>
@@ -2021,7 +2021,7 @@
         <v>4</v>
       </c>
       <c r="AG5" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AH5" t="s">
         <v>4</v>
@@ -2075,7 +2075,7 @@
         <v>52</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>119</v>
@@ -2138,7 +2138,7 @@
         <v>4</v>
       </c>
       <c r="AG6" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AH6" t="s">
         <v>4</v>
@@ -2192,7 +2192,7 @@
         <v>52</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>119</v>
@@ -2255,7 +2255,7 @@
         <v>4</v>
       </c>
       <c r="AG7" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AH7" t="s">
         <v>4</v>
@@ -2302,16 +2302,16 @@
         <v>4</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>154</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>155</v>
       </c>
       <c r="K8" s="2">
         <v>168</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>119</v>
@@ -2353,7 +2353,7 @@
         <v>50</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AA8" s="2">
         <v>5.9999999999999995E-4</v>
@@ -2374,7 +2374,7 @@
         <v>4</v>
       </c>
       <c r="AG8" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AH8" t="s">
         <v>4</v>
@@ -2421,16 +2421,16 @@
         <v>4</v>
       </c>
       <c r="I9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>154</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>155</v>
       </c>
       <c r="K9" s="2">
         <v>168</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>119</v>
@@ -2472,7 +2472,7 @@
         <v>50</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AA9" s="2">
         <v>5.9999999999999995E-4</v>
@@ -2494,7 +2494,7 @@
         <v>4</v>
       </c>
       <c r="AG9" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AH9" t="s">
         <v>4</v>
@@ -2541,16 +2541,16 @@
         <v>4</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K10" s="2">
         <v>1479</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>119</v>
@@ -2613,7 +2613,7 @@
         <v>4</v>
       </c>
       <c r="AG10" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AH10" t="s">
         <v>4</v>
@@ -2660,16 +2660,16 @@
         <v>4</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K11" s="2">
         <v>1479</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>119</v>
@@ -2732,7 +2732,7 @@
         <v>4</v>
       </c>
       <c r="AG11" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AH11" t="s">
         <v>4</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
@@ -2779,14 +2779,14 @@
         <v>4</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2">
         <v>16562</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>119</v>
@@ -2829,7 +2829,7 @@
         <v>0.08</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AA12" s="2">
         <v>1</v>
@@ -2850,7 +2850,7 @@
         <v>4</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AH12" t="s">
         <v>4</v>
@@ -2859,7 +2859,7 @@
         <v>33</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK12" s="2" t="s">
         <v>32</v>
@@ -2873,7 +2873,7 @@
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>31</v>
@@ -2899,14 +2899,14 @@
         <v>4</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2">
         <v>16562</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>119</v>
@@ -2949,7 +2949,7 @@
         <v>0.08</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AA13" s="2">
         <v>1</v>
@@ -2971,7 +2971,7 @@
         <v>4</v>
       </c>
       <c r="AG13" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AH13" t="s">
         <v>4</v>
@@ -2980,7 +2980,7 @@
         <v>33</v>
       </c>
       <c r="AJ13" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK13" s="2" t="s">
         <v>32</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -3020,14 +3020,14 @@
         <v>4</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2">
         <v>16562</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>119</v>
@@ -3070,7 +3070,7 @@
         <v>0.08</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AA14" s="2">
         <v>1</v>
@@ -3092,7 +3092,7 @@
         <v>4</v>
       </c>
       <c r="AG14" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AH14" t="s">
         <v>4</v>
@@ -3101,7 +3101,7 @@
         <v>33</v>
       </c>
       <c r="AJ14" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK14" s="2" t="s">
         <v>32</v>
@@ -3139,16 +3139,16 @@
         <v>4</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K15" s="2">
         <v>46</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>119</v>
@@ -3212,7 +3212,7 @@
         <v>4</v>
       </c>
       <c r="AG15" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AH15" t="s">
         <v>4</v>
@@ -3259,14 +3259,14 @@
         <v>4</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2">
         <v>46</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>119</v>
@@ -3330,7 +3330,7 @@
         <v>4</v>
       </c>
       <c r="AG16" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AH16" t="s">
         <v>4</v>
@@ -3377,14 +3377,14 @@
         <v>4</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2">
         <v>46</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>119</v>
@@ -3448,7 +3448,7 @@
         <v>4</v>
       </c>
       <c r="AG17" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AH17" t="s">
         <v>4</v>
@@ -3495,16 +3495,16 @@
         <v>4</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K18" s="2">
         <v>29</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>43</v>
@@ -3567,7 +3567,7 @@
         <v>4</v>
       </c>
       <c r="AG18" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AH18" s="2" t="s">
         <v>3</v>
@@ -3612,16 +3612,16 @@
         <v>4</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K19" s="2">
         <v>29</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>43</v>
@@ -3684,7 +3684,7 @@
         <v>4</v>
       </c>
       <c r="AG19" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AH19" s="2" t="s">
         <v>3</v>
@@ -3729,16 +3729,16 @@
         <v>4</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K20" s="2">
         <v>29</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>43</v>
@@ -3801,7 +3801,7 @@
         <v>4</v>
       </c>
       <c r="AG20" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AH20" s="2" t="s">
         <v>3</v>
@@ -3846,16 +3846,16 @@
         <v>4</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K21" s="2">
         <v>29</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>43</v>
@@ -3918,7 +3918,7 @@
         <v>4</v>
       </c>
       <c r="AG21" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AH21" s="2" t="s">
         <v>3</v>
@@ -3963,16 +3963,16 @@
         <v>4</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K22" s="2">
         <v>29</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>44</v>
@@ -4035,7 +4035,7 @@
         <v>4</v>
       </c>
       <c r="AG22" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AH22" s="2" t="s">
         <v>3</v>
@@ -4083,19 +4083,19 @@
         <v>107</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K23" s="2">
         <v>169</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O23" s="2">
         <v>0</v>
@@ -4149,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="AF23" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AG23" s="2" t="s">
         <v>49</v>
@@ -4204,19 +4204,19 @@
         <v>107</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K24" s="2">
         <v>169</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O24" s="2">
         <v>0</v>
@@ -4270,7 +4270,7 @@
         <v>0</v>
       </c>
       <c r="AF24" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AG24" s="2" t="s">
         <v>49</v>
@@ -4323,19 +4323,19 @@
         <v>107</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K25" s="2">
         <v>169</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>5</v>
@@ -4371,7 +4371,7 @@
         <v>40</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AA25" s="2">
         <v>8.0000000000000004E-4</v>
@@ -4389,7 +4389,7 @@
         <v>8000</v>
       </c>
       <c r="AF25" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AG25" s="2" t="s">
         <v>49</v>
@@ -4439,19 +4439,19 @@
         <v>3</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K26" s="2">
         <v>2</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>74</v>
@@ -4491,7 +4491,7 @@
         <v>20</v>
       </c>
       <c r="Z26" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AA26" s="2">
         <v>1</v>
@@ -4512,7 +4512,7 @@
         <v>4</v>
       </c>
       <c r="AG26" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AH26" t="s">
         <v>4</v>
@@ -4562,13 +4562,13 @@
         <v>107</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K27" s="2">
         <v>124</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>44</v>
@@ -4631,7 +4631,7 @@
         <v>4</v>
       </c>
       <c r="AG27" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AH27" t="s">
         <v>4</v>
@@ -4640,7 +4640,7 @@
         <v>63</v>
       </c>
       <c r="AJ27" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK27" s="2" t="s">
         <v>64</v>
@@ -4681,13 +4681,13 @@
         <v>107</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K28" s="2">
         <v>124</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>44</v>
@@ -4750,7 +4750,7 @@
         <v>4</v>
       </c>
       <c r="AG28" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AH28" t="s">
         <v>4</v>
@@ -4759,7 +4759,7 @@
         <v>63</v>
       </c>
       <c r="AJ28" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK28" s="2" t="s">
         <v>64</v>
@@ -4800,13 +4800,13 @@
         <v>107</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K29" s="2">
         <v>124</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>44</v>
@@ -4869,7 +4869,7 @@
         <v>4</v>
       </c>
       <c r="AG29" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AH29" t="s">
         <v>4</v>
@@ -4878,7 +4878,7 @@
         <v>63</v>
       </c>
       <c r="AJ29" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK29" s="2" t="s">
         <v>64</v>
@@ -4919,13 +4919,13 @@
         <v>107</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K30" s="2">
         <v>124</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>20</v>
@@ -4988,7 +4988,7 @@
         <v>4</v>
       </c>
       <c r="AG30" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AH30" t="s">
         <v>4</v>
@@ -4997,7 +4997,7 @@
         <v>63</v>
       </c>
       <c r="AJ30" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK30" s="2" t="s">
         <v>64</v>
@@ -5038,13 +5038,13 @@
         <v>107</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K31" s="2">
         <v>124</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>20</v>
@@ -5107,7 +5107,7 @@
         <v>4</v>
       </c>
       <c r="AG31" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AH31" t="s">
         <v>4</v>
@@ -5116,7 +5116,7 @@
         <v>63</v>
       </c>
       <c r="AJ31" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK31" s="2" t="s">
         <v>64</v>
@@ -5157,13 +5157,13 @@
         <v>107</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K32" s="2">
         <v>124</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>20</v>
@@ -5226,7 +5226,7 @@
         <v>4</v>
       </c>
       <c r="AG32" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AH32" t="s">
         <v>4</v>
@@ -5235,7 +5235,7 @@
         <v>63</v>
       </c>
       <c r="AJ32" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK32" s="2" t="s">
         <v>64</v>
@@ -5280,7 +5280,7 @@
         <v>298</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>74</v>
@@ -5344,7 +5344,7 @@
         <v>4</v>
       </c>
       <c r="AG33" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AH33" t="s">
         <v>4</v>
@@ -5353,7 +5353,7 @@
         <v>68</v>
       </c>
       <c r="AJ33" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK33" s="2" t="s">
         <v>64</v>
@@ -5398,7 +5398,7 @@
         <v>298</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>74</v>
@@ -5462,7 +5462,7 @@
         <v>4</v>
       </c>
       <c r="AG34" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AH34" t="s">
         <v>4</v>
@@ -5471,7 +5471,7 @@
         <v>68</v>
       </c>
       <c r="AJ34" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK34" s="2" t="s">
         <v>64</v>
@@ -5516,7 +5516,7 @@
         <v>298</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>74</v>
@@ -5580,7 +5580,7 @@
         <v>4</v>
       </c>
       <c r="AG35" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AH35" t="s">
         <v>4</v>
@@ -5589,7 +5589,7 @@
         <v>68</v>
       </c>
       <c r="AJ35" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK35" s="2" t="s">
         <v>64</v>
@@ -5636,7 +5636,7 @@
         <v>298</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>20</v>
@@ -5700,7 +5700,7 @@
         <v>4</v>
       </c>
       <c r="AG36" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AH36" t="s">
         <v>4</v>
@@ -5709,7 +5709,7 @@
         <v>68</v>
       </c>
       <c r="AJ36" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK36" s="2" t="s">
         <v>64</v>
@@ -5750,13 +5750,13 @@
         <v>107</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K37" s="2">
         <v>165</v>
       </c>
       <c r="L37" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>20</v>
@@ -5819,7 +5819,7 @@
         <v>4</v>
       </c>
       <c r="AG37" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AH37" t="s">
         <v>4</v>
@@ -5869,13 +5869,13 @@
         <v>107</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K38" s="2">
         <v>165</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>20</v>
@@ -5938,7 +5938,7 @@
         <v>4</v>
       </c>
       <c r="AG38" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AH38" t="s">
         <v>4</v>
@@ -5988,13 +5988,13 @@
         <v>107</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K39" s="2">
         <v>165</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>20</v>
@@ -6057,7 +6057,7 @@
         <v>4</v>
       </c>
       <c r="AG39" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AH39" t="s">
         <v>4</v>
@@ -6109,13 +6109,13 @@
         <v>107</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K40" s="2">
         <v>165</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>20</v>
@@ -6178,7 +6178,7 @@
         <v>4</v>
       </c>
       <c r="AG40" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AH40" t="s">
         <v>4</v>
@@ -6228,13 +6228,13 @@
         <v>107</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K41" s="2">
         <v>90</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>20</v>
@@ -6297,7 +6297,7 @@
         <v>4</v>
       </c>
       <c r="AG41" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AH41" t="s">
         <v>4</v>
@@ -6347,19 +6347,19 @@
         <v>107</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K42" s="2">
         <v>10</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O42" s="2">
         <v>0</v>
@@ -6413,7 +6413,7 @@
         <v>0</v>
       </c>
       <c r="AF42" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AG42" s="2" t="s">
         <v>49</v>
@@ -6466,16 +6466,16 @@
         <v>107</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K43" s="2">
         <v>0</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N43" s="2" t="s">
         <v>119</v>
@@ -6535,7 +6535,7 @@
         <v>4</v>
       </c>
       <c r="AG43" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AH43" t="s">
         <v>4</v>
@@ -6587,16 +6587,16 @@
         <v>107</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K44" s="2">
         <v>0</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N44" s="2" t="s">
         <v>119</v>
@@ -6656,7 +6656,7 @@
         <v>4</v>
       </c>
       <c r="AG44" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AH44" t="s">
         <v>4</v>
@@ -6708,16 +6708,16 @@
         <v>107</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K45" s="2">
         <v>0</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>119</v>
@@ -6777,7 +6777,7 @@
         <v>4</v>
       </c>
       <c r="AG45" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AH45" t="s">
         <v>4</v>
@@ -6827,13 +6827,13 @@
         <v>107</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K46" s="2">
         <v>0</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M46" s="2" t="s">
         <v>20</v>
@@ -6896,7 +6896,7 @@
         <v>4</v>
       </c>
       <c r="AG46" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AH46" t="s">
         <v>4</v>
@@ -6946,13 +6946,13 @@
         <v>107</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K47" s="2">
         <v>0</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M47" s="2" t="s">
         <v>20</v>
@@ -7015,7 +7015,7 @@
         <v>4</v>
       </c>
       <c r="AG47" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AH47" t="s">
         <v>4</v>
@@ -7065,13 +7065,13 @@
         <v>107</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K48" s="2">
         <v>5</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M48" s="2" t="s">
         <v>20</v>
@@ -7134,7 +7134,7 @@
         <v>4</v>
       </c>
       <c r="AG48" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AH48" t="s">
         <v>4</v>
@@ -7184,13 +7184,13 @@
         <v>107</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K49" s="2">
         <v>149</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M49" s="2" t="s">
         <v>20</v>
@@ -7253,7 +7253,7 @@
         <v>4</v>
       </c>
       <c r="AG49" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AH49" s="2" t="s">
         <v>3</v>
@@ -7303,13 +7303,13 @@
         <v>107</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K50" s="2">
         <v>44</v>
       </c>
       <c r="L50" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M50" s="2" t="s">
         <v>20</v>
@@ -7422,13 +7422,13 @@
         <v>107</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K51" s="2">
         <v>44</v>
       </c>
       <c r="L51" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M51" s="2" t="s">
         <v>20</v>
@@ -7536,10 +7536,10 @@
         <v>3</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K52" s="2">
         <v>0</v>
@@ -7552,7 +7552,7 @@
         <v>119</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P52" s="2" t="s">
         <v>20</v>
@@ -7606,7 +7606,7 @@
         <v>4</v>
       </c>
       <c r="AG52" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AH52" t="s">
         <v>4</v>
@@ -7653,10 +7653,10 @@
         <v>3</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K53" s="2">
         <v>0</v>
@@ -7669,7 +7669,7 @@
         <v>119</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P53" s="2" t="s">
         <v>20</v>
@@ -7724,7 +7724,7 @@
         <v>4</v>
       </c>
       <c r="AG53" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AH53" t="s">
         <v>4</v>
@@ -7774,7 +7774,7 @@
         <v>107</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K54" s="2">
         <v>0</v>
@@ -7841,7 +7841,7 @@
         <v>4</v>
       </c>
       <c r="AG54" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AH54" t="s">
         <v>4</v>
@@ -7888,16 +7888,16 @@
         <v>4</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K55" s="2">
         <v>7</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M55" s="2" t="s">
         <v>102</v>
@@ -7960,7 +7960,7 @@
         <v>4</v>
       </c>
       <c r="AG55" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AH55" s="2" t="s">
         <v>3</v>
@@ -8007,16 +8007,16 @@
         <v>4</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K56" s="2">
         <v>7</v>
       </c>
       <c r="L56" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M56" s="2" t="s">
         <v>102</v>
@@ -8126,7 +8126,7 @@
         <v>4</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2">
@@ -8194,7 +8194,7 @@
         <v>4</v>
       </c>
       <c r="AG57" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AH57" s="2" t="s">
         <v>3</v>
@@ -8309,7 +8309,7 @@
         <v>4</v>
       </c>
       <c r="AG58" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AH58" s="2" t="s">
         <v>3</v>
@@ -8363,7 +8363,7 @@
         <v>157</v>
       </c>
       <c r="L59" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M59" s="2" t="s">
         <v>111</v>
@@ -8426,7 +8426,7 @@
         <v>4</v>
       </c>
       <c r="AG59" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AH59" t="s">
         <v>4</v>
@@ -8480,7 +8480,7 @@
         <v>157</v>
       </c>
       <c r="L60" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M60" s="2" t="s">
         <v>111</v>
@@ -8543,7 +8543,7 @@
         <v>4</v>
       </c>
       <c r="AG60" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AH60" t="s">
         <v>4</v>
@@ -8597,7 +8597,7 @@
         <v>157</v>
       </c>
       <c r="L61" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M61" s="2" t="s">
         <v>111</v>
@@ -8660,7 +8660,7 @@
         <v>4</v>
       </c>
       <c r="AG61" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AH61" t="s">
         <v>4</v>
@@ -8716,7 +8716,7 @@
         <v>157</v>
       </c>
       <c r="L62" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M62" s="2" t="s">
         <v>20</v>
@@ -8779,7 +8779,7 @@
         <v>4</v>
       </c>
       <c r="AG62" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AH62" t="s">
         <v>4</v>
@@ -8826,7 +8826,7 @@
         <v>4</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2">
@@ -8894,7 +8894,7 @@
         <v>4</v>
       </c>
       <c r="AG63" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AH63" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Bar charts with csv are now split
</commit_message>
<xml_diff>
--- a/src/lib/excels/CI_Comps.xlsx
+++ b/src/lib/excels/CI_Comps.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3960B16-8E25-1A4A-BB2A-584F7A9CFA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{D3960B16-8E25-1A4A-BB2A-584F7A9CFA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21F9DD98-F54C-CD4E-B3CE-39D77ED7FDF6}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{AB0D5E22-6F5B-EC43-9578-14FEE2B3982A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="253">
   <si>
     <t>Packaged</t>
   </si>
@@ -339,9 +339,6 @@
     <t>Yes - Snapshots</t>
   </si>
   <si>
-    <t>Ubuntu, Docker (installed on ubuntu)</t>
-  </si>
-  <si>
     <t>Hercules CI</t>
   </si>
   <si>
@@ -366,12 +363,6 @@
     <t>On-Premises</t>
   </si>
   <si>
-    <t>Docker, Linux VM, Mac VM, Windows VM</t>
-  </si>
-  <si>
-    <t>Linux VM 1GB 1; Container 1GB 2; Windows VM 1GB 2; MacOS VM 1GB 6</t>
-  </si>
-  <si>
     <t>Analytics in Pipeline history - https://buddy.works/docs/pipelines/introduction#pipeline-history</t>
   </si>
   <si>
@@ -765,9 +756,6 @@
     <t>GitHub</t>
   </si>
   <si>
-    <t>GitHub, Bitbucket, AWS CodeCommit, AWS S3</t>
-  </si>
-  <si>
     <t>GitHub, Bitbucket</t>
   </si>
   <si>
@@ -793,6 +781,15 @@
   </si>
   <si>
     <t>PriceExtraUser$</t>
+  </si>
+  <si>
+    <t>GitHub, Bitbucket, AWS CodeCommit</t>
+  </si>
+  <si>
+    <t>Docker, Linux, macOS, Windows</t>
+  </si>
+  <si>
+    <t>Linux VM 1GB 1; Container 1GB 2; Windows VM 1GB 2; macOSOS VM 1GB 6</t>
   </si>
 </sst>
 </file>
@@ -1414,9 +1411,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5061CA7-1C66-674F-BCE4-63FE3AA9D03F}">
   <dimension ref="A1:AM63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD2" sqref="AD2"/>
+      <selection pane="topRight" activeCell="Y44" sqref="Y44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1479,13 +1476,13 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -1497,97 +1494,97 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" t="s">
+        <v>168</v>
+      </c>
+      <c r="M1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O1" t="s">
+        <v>137</v>
+      </c>
+      <c r="P1" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" t="s">
         <v>122</v>
       </c>
-      <c r="J1" t="s">
-        <v>152</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="S1" t="s">
+        <v>132</v>
+      </c>
+      <c r="T1" t="s">
         <v>123</v>
       </c>
-      <c r="L1" t="s">
-        <v>171</v>
-      </c>
-      <c r="M1" t="s">
-        <v>143</v>
-      </c>
-      <c r="N1" t="s">
-        <v>144</v>
-      </c>
-      <c r="O1" t="s">
-        <v>140</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
+        <v>231</v>
+      </c>
+      <c r="V1" t="s">
+        <v>232</v>
+      </c>
+      <c r="W1" t="s">
+        <v>237</v>
+      </c>
+      <c r="X1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA1" t="s">
         <v>124</v>
       </c>
-      <c r="Q1" t="s">
-        <v>139</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="AB1" t="s">
         <v>125</v>
       </c>
-      <c r="S1" t="s">
-        <v>135</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="AC1" t="s">
         <v>126</v>
       </c>
-      <c r="U1" t="s">
-        <v>234</v>
-      </c>
-      <c r="V1" t="s">
-        <v>235</v>
-      </c>
-      <c r="W1" t="s">
-        <v>240</v>
-      </c>
-      <c r="X1" t="s">
-        <v>239</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>241</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>194</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AF1" t="s">
         <v>127</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AG1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH1" t="s">
         <v>128</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AI1" t="s">
+        <v>215</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>129</v>
       </c>
-      <c r="AD1" t="s">
-        <v>253</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AK1" t="s">
+        <v>216</v>
+      </c>
+      <c r="AL1" t="s">
         <v>130</v>
       </c>
-      <c r="AG1" t="s">
-        <v>217</v>
-      </c>
-      <c r="AH1" t="s">
+      <c r="AM1" t="s">
         <v>131</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>218</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>219</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
@@ -1601,10 +1598,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1616,79 +1613,79 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="N2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="O2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="P2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="Q2" t="s">
+        <v>227</v>
+      </c>
+      <c r="R2" t="s">
+        <v>244</v>
+      </c>
+      <c r="S2" t="s">
+        <v>243</v>
+      </c>
+      <c r="T2" t="s">
+        <v>245</v>
+      </c>
+      <c r="U2" t="s">
         <v>230</v>
       </c>
-      <c r="R2" t="s">
-        <v>248</v>
-      </c>
-      <c r="S2" t="s">
-        <v>247</v>
-      </c>
-      <c r="T2" t="s">
-        <v>249</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>233</v>
       </c>
-      <c r="V2" t="s">
-        <v>236</v>
-      </c>
       <c r="W2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="X2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="Y2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AA2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="AB2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AC2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="AD2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AE2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AF2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AH2" t="s">
         <v>26</v>
       </c>
       <c r="AJ2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="AL2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="AM2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.2">
@@ -1717,20 +1714,20 @@
         <v>4</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2">
         <v>1800</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O3" s="2">
         <v>0</v>
@@ -1787,7 +1784,7 @@
         <v>4</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AH3" t="s">
         <v>4</v>
@@ -1834,17 +1831,17 @@
         <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2">
         <v>52</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>20</v>
@@ -1883,7 +1880,7 @@
         <v>50</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AA4" s="2">
         <v>5.9999999999999995E-4</v>
@@ -1904,7 +1901,7 @@
         <v>4</v>
       </c>
       <c r="AG4" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AH4" t="s">
         <v>4</v>
@@ -1951,17 +1948,17 @@
         <v>3</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2">
         <v>52</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>20</v>
@@ -2000,7 +1997,7 @@
         <v>50</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AA5" s="2">
         <v>5.9999999999999995E-4</v>
@@ -2021,7 +2018,7 @@
         <v>4</v>
       </c>
       <c r="AG5" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AH5" t="s">
         <v>4</v>
@@ -2068,17 +2065,17 @@
         <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2">
         <v>52</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>20</v>
@@ -2117,7 +2114,7 @@
         <v>50</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AA6" s="2">
         <v>5.9999999999999995E-4</v>
@@ -2138,7 +2135,7 @@
         <v>4</v>
       </c>
       <c r="AG6" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AH6" t="s">
         <v>4</v>
@@ -2185,17 +2182,17 @@
         <v>3</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2">
         <v>52</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>20</v>
@@ -2234,7 +2231,7 @@
         <v>50</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AA7" s="2">
         <v>5.9999999999999995E-4</v>
@@ -2255,7 +2252,7 @@
         <v>4</v>
       </c>
       <c r="AG7" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AH7" t="s">
         <v>4</v>
@@ -2302,22 +2299,22 @@
         <v>4</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K8" s="2">
         <v>168</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O8" s="2">
         <v>30</v>
@@ -2353,7 +2350,7 @@
         <v>50</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AA8" s="2">
         <v>5.9999999999999995E-4</v>
@@ -2374,7 +2371,7 @@
         <v>4</v>
       </c>
       <c r="AG8" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="AH8" t="s">
         <v>4</v>
@@ -2421,22 +2418,22 @@
         <v>4</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K9" s="2">
         <v>168</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O9" s="2">
         <v>80</v>
@@ -2472,7 +2469,7 @@
         <v>50</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AA9" s="2">
         <v>5.9999999999999995E-4</v>
@@ -2494,7 +2491,7 @@
         <v>4</v>
       </c>
       <c r="AG9" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="AH9" t="s">
         <v>4</v>
@@ -2541,22 +2538,22 @@
         <v>4</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K10" s="2">
         <v>1479</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O10" s="2">
         <v>1</v>
@@ -2613,7 +2610,7 @@
         <v>4</v>
       </c>
       <c r="AG10" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="AH10" t="s">
         <v>4</v>
@@ -2660,22 +2657,22 @@
         <v>4</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K11" s="2">
         <v>1479</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O11" s="4">
         <v>1</v>
@@ -2732,7 +2729,7 @@
         <v>4</v>
       </c>
       <c r="AG11" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="AH11" t="s">
         <v>4</v>
@@ -2755,7 +2752,7 @@
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
@@ -2779,20 +2776,20 @@
         <v>4</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2">
         <v>16562</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>5</v>
@@ -2829,7 +2826,7 @@
         <v>0.08</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="AA12" s="2">
         <v>1</v>
@@ -2850,7 +2847,7 @@
         <v>4</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AH12" t="s">
         <v>4</v>
@@ -2859,7 +2856,7 @@
         <v>33</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK12" s="2" t="s">
         <v>32</v>
@@ -2873,7 +2870,7 @@
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>31</v>
@@ -2899,20 +2896,20 @@
         <v>4</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2">
         <v>16562</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>5</v>
@@ -2949,7 +2946,7 @@
         <v>0.08</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="AA13" s="2">
         <v>1</v>
@@ -2971,7 +2968,7 @@
         <v>4</v>
       </c>
       <c r="AG13" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AH13" t="s">
         <v>4</v>
@@ -2980,7 +2977,7 @@
         <v>33</v>
       </c>
       <c r="AJ13" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK13" s="2" t="s">
         <v>32</v>
@@ -2994,7 +2991,7 @@
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
@@ -3020,20 +3017,20 @@
         <v>4</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2">
         <v>16562</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>5</v>
@@ -3070,7 +3067,7 @@
         <v>0.08</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="AA14" s="2">
         <v>1</v>
@@ -3092,7 +3089,7 @@
         <v>4</v>
       </c>
       <c r="AG14" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AH14" t="s">
         <v>4</v>
@@ -3101,7 +3098,7 @@
         <v>33</v>
       </c>
       <c r="AJ14" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK14" s="2" t="s">
         <v>32</v>
@@ -3139,22 +3136,22 @@
         <v>4</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K15" s="2">
         <v>46</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>5</v>
@@ -3212,7 +3209,7 @@
         <v>4</v>
       </c>
       <c r="AG15" s="10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AH15" t="s">
         <v>4</v>
@@ -3259,20 +3256,20 @@
         <v>4</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2">
         <v>46</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>5</v>
@@ -3330,7 +3327,7 @@
         <v>4</v>
       </c>
       <c r="AG16" s="10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AH16" t="s">
         <v>4</v>
@@ -3377,20 +3374,20 @@
         <v>4</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2">
         <v>46</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>5</v>
@@ -3448,7 +3445,7 @@
         <v>4</v>
       </c>
       <c r="AG17" s="10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AH17" t="s">
         <v>4</v>
@@ -3495,16 +3492,16 @@
         <v>4</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K18" s="2">
         <v>29</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>43</v>
@@ -3567,7 +3564,7 @@
         <v>4</v>
       </c>
       <c r="AG18" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AH18" s="2" t="s">
         <v>3</v>
@@ -3612,16 +3609,16 @@
         <v>4</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K19" s="2">
         <v>29</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>43</v>
@@ -3684,7 +3681,7 @@
         <v>4</v>
       </c>
       <c r="AG19" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AH19" s="2" t="s">
         <v>3</v>
@@ -3729,16 +3726,16 @@
         <v>4</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K20" s="2">
         <v>29</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>43</v>
@@ -3801,7 +3798,7 @@
         <v>4</v>
       </c>
       <c r="AG20" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AH20" s="2" t="s">
         <v>3</v>
@@ -3846,16 +3843,16 @@
         <v>4</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K21" s="2">
         <v>29</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>43</v>
@@ -3918,7 +3915,7 @@
         <v>4</v>
       </c>
       <c r="AG21" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AH21" s="2" t="s">
         <v>3</v>
@@ -3963,16 +3960,16 @@
         <v>4</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K22" s="2">
         <v>29</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>44</v>
@@ -4035,7 +4032,7 @@
         <v>4</v>
       </c>
       <c r="AG22" s="10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AH22" s="2" t="s">
         <v>3</v>
@@ -4080,22 +4077,22 @@
         <v>4</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K23" s="2">
         <v>169</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="O23" s="2">
         <v>0</v>
@@ -4149,7 +4146,7 @@
         <v>0</v>
       </c>
       <c r="AF23" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="AG23" s="2" t="s">
         <v>49</v>
@@ -4201,22 +4198,22 @@
         <v>4</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K24" s="2">
         <v>169</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="O24" s="2">
         <v>0</v>
@@ -4270,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="AF24" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="AG24" s="2" t="s">
         <v>49</v>
@@ -4320,22 +4317,22 @@
         <v>4</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K25" s="2">
         <v>169</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>5</v>
@@ -4371,7 +4368,7 @@
         <v>40</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AA25" s="2">
         <v>8.0000000000000004E-4</v>
@@ -4389,7 +4386,7 @@
         <v>8000</v>
       </c>
       <c r="AF25" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="AG25" s="2" t="s">
         <v>49</v>
@@ -4439,19 +4436,19 @@
         <v>3</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K26" s="2">
         <v>2</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>74</v>
@@ -4491,7 +4488,7 @@
         <v>20</v>
       </c>
       <c r="Z26" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AA26" s="2">
         <v>1</v>
@@ -4512,7 +4509,7 @@
         <v>4</v>
       </c>
       <c r="AG26" s="10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AH26" t="s">
         <v>4</v>
@@ -4559,16 +4556,16 @@
         <v>4</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K27" s="2">
         <v>124</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>44</v>
@@ -4631,7 +4628,7 @@
         <v>4</v>
       </c>
       <c r="AG27" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AH27" t="s">
         <v>4</v>
@@ -4640,7 +4637,7 @@
         <v>63</v>
       </c>
       <c r="AJ27" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK27" s="2" t="s">
         <v>64</v>
@@ -4678,16 +4675,16 @@
         <v>4</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K28" s="2">
         <v>124</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>44</v>
@@ -4750,7 +4747,7 @@
         <v>4</v>
       </c>
       <c r="AG28" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AH28" t="s">
         <v>4</v>
@@ -4759,7 +4756,7 @@
         <v>63</v>
       </c>
       <c r="AJ28" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK28" s="2" t="s">
         <v>64</v>
@@ -4797,16 +4794,16 @@
         <v>4</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K29" s="2">
         <v>124</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>44</v>
@@ -4869,7 +4866,7 @@
         <v>4</v>
       </c>
       <c r="AG29" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AH29" t="s">
         <v>4</v>
@@ -4878,7 +4875,7 @@
         <v>63</v>
       </c>
       <c r="AJ29" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK29" s="2" t="s">
         <v>64</v>
@@ -4916,16 +4913,16 @@
         <v>4</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K30" s="2">
         <v>124</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>20</v>
@@ -4988,7 +4985,7 @@
         <v>4</v>
       </c>
       <c r="AG30" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AH30" t="s">
         <v>4</v>
@@ -4997,7 +4994,7 @@
         <v>63</v>
       </c>
       <c r="AJ30" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK30" s="2" t="s">
         <v>64</v>
@@ -5035,16 +5032,16 @@
         <v>4</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K31" s="2">
         <v>124</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>20</v>
@@ -5107,7 +5104,7 @@
         <v>4</v>
       </c>
       <c r="AG31" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AH31" t="s">
         <v>4</v>
@@ -5116,7 +5113,7 @@
         <v>63</v>
       </c>
       <c r="AJ31" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK31" s="2" t="s">
         <v>64</v>
@@ -5154,16 +5151,16 @@
         <v>4</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K32" s="2">
         <v>124</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>20</v>
@@ -5226,7 +5223,7 @@
         <v>4</v>
       </c>
       <c r="AG32" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AH32" t="s">
         <v>4</v>
@@ -5235,7 +5232,7 @@
         <v>63</v>
       </c>
       <c r="AJ32" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK32" s="2" t="s">
         <v>64</v>
@@ -5280,13 +5277,13 @@
         <v>298</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>74</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O33" s="2" t="s">
         <v>5</v>
@@ -5344,7 +5341,7 @@
         <v>4</v>
       </c>
       <c r="AG33" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AH33" t="s">
         <v>4</v>
@@ -5353,7 +5350,7 @@
         <v>68</v>
       </c>
       <c r="AJ33" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK33" s="2" t="s">
         <v>64</v>
@@ -5398,13 +5395,13 @@
         <v>298</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>74</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O34" s="2" t="s">
         <v>5</v>
@@ -5462,7 +5459,7 @@
         <v>4</v>
       </c>
       <c r="AG34" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AH34" t="s">
         <v>4</v>
@@ -5471,7 +5468,7 @@
         <v>68</v>
       </c>
       <c r="AJ34" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK34" s="2" t="s">
         <v>64</v>
@@ -5516,13 +5513,13 @@
         <v>298</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>74</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O35" s="2" t="s">
         <v>5</v>
@@ -5580,7 +5577,7 @@
         <v>4</v>
       </c>
       <c r="AG35" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AH35" t="s">
         <v>4</v>
@@ -5589,7 +5586,7 @@
         <v>68</v>
       </c>
       <c r="AJ35" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK35" s="2" t="s">
         <v>64</v>
@@ -5636,13 +5633,13 @@
         <v>298</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O36" s="2">
         <v>0</v>
@@ -5700,7 +5697,7 @@
         <v>4</v>
       </c>
       <c r="AG36" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AH36" t="s">
         <v>4</v>
@@ -5709,7 +5706,7 @@
         <v>68</v>
       </c>
       <c r="AJ36" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AK36" s="2" t="s">
         <v>64</v>
@@ -5747,22 +5744,22 @@
         <v>4</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K37" s="2">
         <v>165</v>
       </c>
       <c r="L37" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O37" s="2">
         <v>0</v>
@@ -5819,7 +5816,7 @@
         <v>4</v>
       </c>
       <c r="AG37" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="AH37" t="s">
         <v>4</v>
@@ -5866,22 +5863,22 @@
         <v>4</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K38" s="2">
         <v>165</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O38" s="2">
         <v>0</v>
@@ -5938,7 +5935,7 @@
         <v>4</v>
       </c>
       <c r="AG38" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="AH38" t="s">
         <v>4</v>
@@ -5985,22 +5982,22 @@
         <v>4</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K39" s="2">
         <v>165</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O39" s="2">
         <v>0</v>
@@ -6057,7 +6054,7 @@
         <v>4</v>
       </c>
       <c r="AG39" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="AH39" t="s">
         <v>4</v>
@@ -6106,22 +6103,22 @@
         <v>4</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K40" s="2">
         <v>165</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O40" s="2">
         <v>0</v>
@@ -6178,7 +6175,7 @@
         <v>4</v>
       </c>
       <c r="AG40" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="AH40" t="s">
         <v>4</v>
@@ -6225,16 +6222,16 @@
         <v>4</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K41" s="2">
         <v>90</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>20</v>
@@ -6297,7 +6294,7 @@
         <v>4</v>
       </c>
       <c r="AG41" s="10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AH41" t="s">
         <v>4</v>
@@ -6344,22 +6341,22 @@
         <v>4</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K42" s="2">
         <v>10</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="O42" s="2">
         <v>0</v>
@@ -6413,7 +6410,7 @@
         <v>0</v>
       </c>
       <c r="AF42" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="AG42" s="2" t="s">
         <v>49</v>
@@ -6463,22 +6460,22 @@
         <v>4</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K43" s="2">
         <v>0</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O43" s="2">
         <v>1</v>
@@ -6535,7 +6532,7 @@
         <v>4</v>
       </c>
       <c r="AG43" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AH43" t="s">
         <v>4</v>
@@ -6584,22 +6581,22 @@
         <v>4</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K44" s="2">
         <v>0</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O44" s="2">
         <v>1</v>
@@ -6656,7 +6653,7 @@
         <v>4</v>
       </c>
       <c r="AG44" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AH44" t="s">
         <v>4</v>
@@ -6705,22 +6702,22 @@
         <v>4</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K45" s="2">
         <v>0</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O45" s="2">
         <v>2</v>
@@ -6777,7 +6774,7 @@
         <v>4</v>
       </c>
       <c r="AG45" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AH45" t="s">
         <v>4</v>
@@ -6824,22 +6821,22 @@
         <v>4</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K46" s="2">
         <v>0</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M46" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O46" s="2" t="s">
         <v>5</v>
@@ -6896,7 +6893,7 @@
         <v>4</v>
       </c>
       <c r="AG46" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AH46" t="s">
         <v>4</v>
@@ -6943,22 +6940,22 @@
         <v>4</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K47" s="2">
         <v>0</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M47" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O47" s="2" t="s">
         <v>5</v>
@@ -7015,7 +7012,7 @@
         <v>4</v>
       </c>
       <c r="AG47" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AH47" t="s">
         <v>4</v>
@@ -7062,22 +7059,22 @@
         <v>4</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K48" s="2">
         <v>5</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="M48" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O48" s="2">
         <v>0</v>
@@ -7134,7 +7131,7 @@
         <v>4</v>
       </c>
       <c r="AG48" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AH48" t="s">
         <v>4</v>
@@ -7181,16 +7178,16 @@
         <v>4</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K49" s="2">
         <v>149</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="M49" s="2" t="s">
         <v>20</v>
@@ -7253,7 +7250,7 @@
         <v>4</v>
       </c>
       <c r="AG49" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AH49" s="2" t="s">
         <v>3</v>
@@ -7300,22 +7297,22 @@
         <v>4</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K50" s="2">
         <v>44</v>
       </c>
       <c r="L50" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M50" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O50" s="2">
         <v>0</v>
@@ -7419,22 +7416,22 @@
         <v>4</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K51" s="2">
         <v>44</v>
       </c>
       <c r="L51" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M51" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O51" s="2">
         <v>0</v>
@@ -7536,23 +7533,23 @@
         <v>3</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K52" s="2">
         <v>0</v>
       </c>
       <c r="L52" s="2"/>
       <c r="M52" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P52" s="2" t="s">
         <v>20</v>
@@ -7606,7 +7603,7 @@
         <v>4</v>
       </c>
       <c r="AG52" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AH52" t="s">
         <v>4</v>
@@ -7653,23 +7650,23 @@
         <v>3</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K53" s="2">
         <v>0</v>
       </c>
       <c r="L53" s="2"/>
       <c r="M53" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P53" s="2" t="s">
         <v>20</v>
@@ -7724,7 +7721,7 @@
         <v>4</v>
       </c>
       <c r="AG53" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AH53" t="s">
         <v>4</v>
@@ -7771,10 +7768,10 @@
         <v>3</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K54" s="2">
         <v>0</v>
@@ -7841,7 +7838,7 @@
         <v>4</v>
       </c>
       <c r="AG54" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AH54" t="s">
         <v>4</v>
@@ -7888,19 +7885,19 @@
         <v>4</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K55" s="2">
         <v>7</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="N55" s="2" t="s">
         <v>20</v>
@@ -7960,7 +7957,7 @@
         <v>4</v>
       </c>
       <c r="AG55" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AH55" s="2" t="s">
         <v>3</v>
@@ -8007,19 +8004,19 @@
         <v>4</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K56" s="2">
         <v>7</v>
       </c>
       <c r="L56" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>20</v>
@@ -8102,10 +8099,10 @@
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="C57">
         <v>55</v>
@@ -8126,7 +8123,7 @@
         <v>4</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2">
@@ -8137,7 +8134,7 @@
         <v>20</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O57" s="2">
         <v>0</v>
@@ -8194,7 +8191,7 @@
         <v>4</v>
       </c>
       <c r="AG57" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AH57" s="2" t="s">
         <v>3</v>
@@ -8217,7 +8214,7 @@
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>13</v>
@@ -8241,7 +8238,7 @@
         <v>3</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2">
@@ -8309,7 +8306,7 @@
         <v>4</v>
       </c>
       <c r="AG58" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AH58" s="2" t="s">
         <v>3</v>
@@ -8332,7 +8329,7 @@
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>13</v>
@@ -8356,17 +8353,17 @@
         <v>4</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J59" s="2"/>
       <c r="K59" s="2">
         <v>157</v>
       </c>
       <c r="L59" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>111</v>
+        <v>251</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>20</v>
@@ -8405,40 +8402,40 @@
         <v>6</v>
       </c>
       <c r="Z59" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB59" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC59" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD59" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE59" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG59" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="AH59" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI59" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AA59" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB59" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC59" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD59" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE59" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF59" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG59" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="AH59" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI59" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="AJ59" t="s">
         <v>4</v>
       </c>
       <c r="AK59" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AL59" s="2" t="s">
         <v>3</v>
@@ -8449,7 +8446,7 @@
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>42</v>
@@ -8473,17 +8470,17 @@
         <v>4</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J60" s="2"/>
       <c r="K60" s="2">
         <v>157</v>
       </c>
       <c r="L60" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>111</v>
+        <v>251</v>
       </c>
       <c r="N60" s="2" t="s">
         <v>20</v>
@@ -8522,7 +8519,7 @@
         <v>6</v>
       </c>
       <c r="Z60" s="2" t="s">
-        <v>112</v>
+        <v>252</v>
       </c>
       <c r="AA60" s="2">
         <v>1.5E-3</v>
@@ -8543,19 +8540,19 @@
         <v>4</v>
       </c>
       <c r="AG60" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AH60" t="s">
         <v>4</v>
       </c>
       <c r="AI60" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AJ60" t="s">
         <v>4</v>
       </c>
       <c r="AK60" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AL60" s="2" t="s">
         <v>3</v>
@@ -8566,10 +8563,10 @@
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="C61">
         <v>59</v>
@@ -8590,17 +8587,17 @@
         <v>4</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2">
         <v>157</v>
       </c>
       <c r="L61" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>111</v>
+        <v>251</v>
       </c>
       <c r="N61" s="2" t="s">
         <v>20</v>
@@ -8639,7 +8636,7 @@
         <v>6</v>
       </c>
       <c r="Z61" s="2" t="s">
-        <v>112</v>
+        <v>252</v>
       </c>
       <c r="AA61" s="2">
         <v>1.5E-3</v>
@@ -8660,19 +8657,19 @@
         <v>4</v>
       </c>
       <c r="AG61" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AH61" t="s">
         <v>4</v>
       </c>
       <c r="AI61" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AJ61" t="s">
         <v>4</v>
       </c>
       <c r="AK61" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AL61" s="2" t="s">
         <v>3</v>
@@ -8683,10 +8680,10 @@
     </row>
     <row r="62" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C62">
         <v>60</v>
@@ -8709,20 +8706,20 @@
         <v>4</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2">
         <v>157</v>
       </c>
       <c r="L62" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="M62" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>111</v>
+        <v>251</v>
       </c>
       <c r="O62" s="2">
         <v>0</v>
@@ -8779,19 +8776,19 @@
         <v>4</v>
       </c>
       <c r="AG62" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AH62" t="s">
         <v>4</v>
       </c>
       <c r="AI62" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AJ62" t="s">
         <v>4</v>
       </c>
       <c r="AK62" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AL62" s="2" t="s">
         <v>3</v>
@@ -8802,7 +8799,7 @@
     </row>
     <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>66</v>
@@ -8826,7 +8823,7 @@
         <v>4</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2">
@@ -8834,7 +8831,7 @@
       </c>
       <c r="L63" s="2"/>
       <c r="M63" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N63" s="2" t="s">
         <v>20</v>
@@ -8894,19 +8891,19 @@
         <v>4</v>
       </c>
       <c r="AG63" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AH63" t="s">
         <v>4</v>
       </c>
       <c r="AI63" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AJ63" t="s">
         <v>4</v>
       </c>
       <c r="AK63" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AL63" s="2" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Added dollar sign to final price, changed GitHub platforms from "Other" to "All" because it was confusing;
</commit_message>
<xml_diff>
--- a/src/lib/excels/CI_Comps.xlsx
+++ b/src/lib/excels/CI_Comps.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{D3960B16-8E25-1A4A-BB2A-584F7A9CFA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39639059-0FF9-CC4B-A29D-4CB9EE66B8D1}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{D3960B16-8E25-1A4A-BB2A-584F7A9CFA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9BC3F60-7D3F-8648-B0D1-D6C4FCE7047E}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{AB0D5E22-6F5B-EC43-9578-14FEE2B3982A}"/>
   </bookViews>
@@ -771,9 +771,6 @@
     <t>Linux 2CPU: 0.008;Docker 2CPU: 0.008; macOS 3CPU: 0.08; Windows 2CPU: 0.016; https://docs.github.com/en/actions/hosting-your-own-runners/about-self-hosted-runners#requirements-for-self-hosted-runner-machines</t>
   </si>
   <si>
-    <t>Final Price</t>
-  </si>
-  <si>
     <t>Not controllable</t>
   </si>
   <si>
@@ -793,6 +790,9 @@
   </si>
   <si>
     <t>Extras Included</t>
+  </si>
+  <si>
+    <t>Final Price $</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1065,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1420,7 +1416,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1492,7 +1488,7 @@
         <v>146</v>
       </c>
       <c r="F1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1564,7 +1560,7 @@
         <v>125</v>
       </c>
       <c r="AD1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AE1" t="s">
         <v>132</v>
@@ -1608,10 +1604,10 @@
         <v>147</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="F2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -4153,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="AF23" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG23" s="2" t="s">
         <v>48</v>
@@ -4274,7 +4270,7 @@
         <v>0</v>
       </c>
       <c r="AF24" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG24" s="2" t="s">
         <v>48</v>
@@ -4393,7 +4389,7 @@
         <v>8000</v>
       </c>
       <c r="AF25" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG25" s="2" t="s">
         <v>48</v>
@@ -4443,7 +4439,7 @@
         <v>2</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>156</v>
@@ -6417,7 +6413,7 @@
         <v>0</v>
       </c>
       <c r="AF42" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG42" s="2" t="s">
         <v>48</v>
@@ -8370,7 +8366,7 @@
         <v>185</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>19</v>
@@ -8409,7 +8405,7 @@
         <v>6</v>
       </c>
       <c r="Z59" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AA59" s="2" t="s">
         <v>19</v>
@@ -8487,7 +8483,7 @@
         <v>185</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N60" s="2" t="s">
         <v>19</v>
@@ -8526,7 +8522,7 @@
         <v>6</v>
       </c>
       <c r="Z60" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AA60" s="2">
         <v>1.5E-3</v>
@@ -8604,7 +8600,7 @@
         <v>185</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N61" s="2" t="s">
         <v>19</v>
@@ -8643,7 +8639,7 @@
         <v>6</v>
       </c>
       <c r="Z61" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AA61" s="2">
         <v>1.5E-3</v>
@@ -8726,7 +8722,7 @@
         <v>19</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O62" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Final price to monthly price
</commit_message>
<xml_diff>
--- a/src/lib/excels/CI_Comps.xlsx
+++ b/src/lib/excels/CI_Comps.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{D3960B16-8E25-1A4A-BB2A-584F7A9CFA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9BC3F60-7D3F-8648-B0D1-D6C4FCE7047E}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{D3960B16-8E25-1A4A-BB2A-584F7A9CFA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3001CEF3-6DCE-F34A-8BD7-938E2F304C41}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{AB0D5E22-6F5B-EC43-9578-14FEE2B3982A}"/>
   </bookViews>
@@ -792,7 +792,7 @@
     <t>Extras Included</t>
   </si>
   <si>
-    <t>Final Price $</t>
+    <t>Monthly Price $</t>
   </si>
 </sst>
 </file>
@@ -1065,6 +1065,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1415,8 +1419,8 @@
   <dimension ref="A1:AM63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>